<commit_message>
Secton KPI added, Electricity and Petrol consumption files added
</commit_message>
<xml_diff>
--- a/ESG-temp.xlsx
+++ b/ESG-temp.xlsx
@@ -14,111 +14,191 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
-  <si>
-    <t>Region</t>
-  </si>
-  <si>
-    <t>Local Authority</t>
-  </si>
-  <si>
-    <t>Geographic Code</t>
-  </si>
-  <si>
-    <t>Unnamed: 3</t>
-  </si>
-  <si>
-    <t>Factories</t>
-  </si>
-  <si>
-    <t>Unnamed: 5</t>
-  </si>
-  <si>
-    <t>Unnamed: 6</t>
-  </si>
-  <si>
-    <t>Unnamed: 7</t>
-  </si>
-  <si>
-    <t>Unnamed: 8</t>
-  </si>
-  <si>
-    <t>Offices</t>
-  </si>
-  <si>
-    <t>Unnamed: 10</t>
-  </si>
-  <si>
-    <t>Unnamed: 11</t>
-  </si>
-  <si>
-    <t>Unnamed: 12</t>
-  </si>
-  <si>
-    <t>Unnamed: 13</t>
-  </si>
-  <si>
-    <t>Shops</t>
-  </si>
-  <si>
-    <t>Unnamed: 15</t>
-  </si>
-  <si>
-    <t>Unnamed: 16</t>
-  </si>
-  <si>
-    <t>Unnamed: 17</t>
-  </si>
-  <si>
-    <t>Unnamed: 18</t>
-  </si>
-  <si>
-    <t>Warehouses</t>
-  </si>
-  <si>
-    <t>Unnamed: 20</t>
-  </si>
-  <si>
-    <t>Unnamed: 21</t>
-  </si>
-  <si>
-    <t>Unnamed: 22</t>
-  </si>
-  <si>
-    <t>Unnamed: 23</t>
-  </si>
-  <si>
-    <t>All other sectors</t>
-  </si>
-  <si>
-    <t>Unnamed: 25</t>
-  </si>
-  <si>
-    <t>Unnamed: 26</t>
-  </si>
-  <si>
-    <t>Unnamed: 27</t>
-  </si>
-  <si>
-    <t>Unnamed: 28</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>Unnamed: 30</t>
-  </si>
-  <si>
-    <t>Unnamed: 31</t>
-  </si>
-  <si>
-    <t>Unnamed: 32</t>
-  </si>
-  <si>
-    <t>North East</t>
-  </si>
-  <si>
-    <t>E12000001</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t>Factory</t>
+  </si>
+  <si>
+    <t>Office</t>
+  </si>
+  <si>
+    <t>Shop</t>
+  </si>
+  <si>
+    <t>Warehouse</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>[0.4156188619777074 0.23405098838021451 0.3548069747178907
+ 0.3925789782501215 0.26500711687780437 0.23808662088552426
+ 0.3227003667363439 0.3702002602385826 0.2690201233575771
+ 0.2560234357101133 0.3314833454396688 0.3742499337403722
+ 0.4722202598164068 0.2826696029378756 0.39007078537107454
+ 0.18599860987939326 0.30961227659283513 0.2538735680625153
+ 0.35081719329128785 0.28157518120276875 0.28412914452448107
+ 0.23848833485857018 0.24239089748901912 0.21322682517773087
+ 0.3072724212036131 0.25807691764475904 0.23874832353994388
+ 0.37296948568927757 0.3528159696778007 0.22030347709445666
+ 0.17344026337921586 0.12613924342182847 0.3864029388352233
+ 0.4724498829432705 0.18913560651080433 0.2945501937970353
+ 0.30554938203832577 0.41851596736813235 0.1990144769925904
+ 0.20717365057303788 0.30434168919330046 0.2686350808033585
+ 0.2845758833817538 0.2320433463267217 0.4093837290932118
+ 0.21186443924500595 0.13585499279556068 0.3590855954964528
+ 0.34881705862577467 0.2808228580521429 0.34049300866674176
+ 0.38428767323064245 0.34538244050219585 0.3720840332469437
+ 0.34911183208981594 0.22699830195391327 0.30112832812381973
+ 0.33680075996470976 0.2113660124625376 0.3691590757829753
+ 0.4137309062424565 0.23897712281419167 0.25623394599065324
+ 0.2854264370275957 0.22940021942561512 0.4053404306589977
+ 0.3242270677809528 0.305004636918721 0.28377348125301866
+ 0.30416111896330367 0.24284935187962026 0.21059260470156269
+ 0.4680873488923975 0.4007022070074062 0.2858982841916463
+ 0.18549949133779417 0.29573339188436915 0.39643621228270587
+ 0.469043468348977 0.3728275879965346 0.3170626418980237
+ 0.32146395933741756 0.1605763541619129 0.3761144632244019
+ 0.35860237630179975 0.29419087980746167 0.19249808491898512
+ 0.4043988078127421 0.2704431919271187 0.12400638747216508
+ 0.4097333943538327 0.3333370143496294 0.3338122202520238
+ 0.3878839799925342 0.23585728339224754 0.35329789744679324
+ 0.3742948064903305 0.2576888234186233 0.44372819994231144
+ 0.306762397077868 0.20330495217552397 0.1778415068769707
+ 0.2160226336838365 0.37992471646279347 0.3220222735132056
+ 0.3313055969992261 0.30185930300308245 0.3688067348707397
+ 0.2993225765087857 0.2392105024816921 0.2603552790380365
+ 0.2712397207609811 0.24723627154112815 0.21725471880964653
+ 0.3062804311983664 0.2797181819920004 0.3527259485963495
+ 0.2885773105547127 0.3508067182166133 0.24788083319405418
+ 0.3125472792099555 0.19313861784376568 0.18989890845612092
+ 0.2860365898177573 0.43581104868820997 0.2919970777557367
+ 0.3724991365840005 0.2850390539209088 0.09062680772356257
+ 0.3728485887741661 0.24422220768134953 0.4201343542894879
+ 0.28388502279446254 0.21403279911391895 0.2530849997289014
+ 0.4784823914906977 0.32745685574678646 0.24154256253024667
+ 0.35834607758902565 0.31568443141815206 0.2660111338353016
+ 0.31067954144494286 0.33531109183692037 0.3036163045043696
+ 0.21392709806347496 0.2760913062048397 0.3233870366172847
+ 0.11251554731189832 0.2950756348100071 0.29368813543661526
+ 0.09197741307262461 0.2505321337579612 0.1946519464301338
+ 0.17923372520357947 0.16787699213551882 0.08412800475552175
+ 0.23655727680751348 0.29174218931121637 0.22910243966786706
+ 0.18554298073835163 0.4036672959293843 0.22559335188941848
+ 0.2992193320667802 0.07286912225730753 0.32853170320730996
+ 0.12437732082255329 0.29655190995879993 0.24152247837080493
+ 0.36228963211638626 0.3286641951012646 0.26585982107638984
+ 0.3106234915689516 0.23024817736531508 0.2129584072527725
+ 0.23941853864741122 0.22396334152666642 0.28001853526264037
+ 0.17423808493361984 0.0826137646796217 0.34214498678167526
+ 0.2265435872056051 0.14397694525508445 0.1504775090840921
+ 0.19860566161089677 0.1357199797230446 0.16190632936477928
+ 0.2954233314963489 0.09302322399298268 0.04504459828634631
+ 0.21704838769074 0.11498628961256795 0.09709334532685222
+ 0.03640706170896144 0.00024533702965647653 0.10078084140831398
+ 0.16371610647634113 0.12247082139320116 0.11763680094873316
+ 0.15606990285490382 0.04854964833612459 0.1644852153351857
+ 0.15277350007556478 0.10418156464669223 0.10200122849442023
+ 0.11613980906324108 0.05896888515445104 0.028356996112661986
+ 0.05997711723204742 0.11532636112822503 0.10827519730775334
+ 0.15791664540712894 0.15578726809727525 0.12247495681454308
+ 0.07233427541410038 0.09325474516453716 0.08909188428205235
+ 0.06414417325094483 0.16662165362771195 0.10128293918811992
+ 0.0021686686275121793 0.28874047412923665 0.23859884325487551
+ 0.2522366250801507 0.19572749687039423 0.06293491618587886
+ 0.10232409259860366 0.22395524620814072 0.16837390086427315
+ 0.25519479828554836 0.2567299097187502 0.12535987183565891
+ 0.09086201754566968 0.1651137742543603 0.34147277364626405
+ 0.1604697683326993 0.3022776423454536 0.1484359878763141
+ 0.06189016589444755 0.2638364214255791 0.17555294771449545
+ 0.35268782744440036 0.1871415742189123 0.12515961549185542
+ 0.18106793886628592 0.26519713620381474 0.3048032088860423
+ 0.19848911014042658 0.31733956019463744 0.22917558309519118
+ 0.18424563653074078 0.2401096801748096 0.19187960085252867
+ 0.162873507500126 0.14921353325163111 0.20533540440837533
+ 0.0608151995201832 0.2494216111533808 0.1144181208772027
+ 0.1102609870992895 0.18078157560672106 0.08003252641972185
+ 0.17741607362535386 0.17428238981020086 0.1640503546037345
+ 0.171434467951431 0.1445160457366755 0.09435621105226151
+ 0.16184075464085032 0.1820441430017142 0.1433512701121092
+ 0.26984159241152034 0.22891212114427384 0.1517262498247298
+ 0.10732472481509608 0.23761217731808715 0.1580315785654259
+ 0.20289846520186897 0.13566809557174717 0.318216437940199
+ 0.21852999589218883 0.16227444949366915 0.1395969025617612
+ 0.12655340092698739 0.20435770190266947 0.2034785248443057
+ 0.2772856589751561 0.13700347606239272 0.22393403494658387
+ 0.2500560547300013 0.22504145762959882 0.36172256460409985
+ 0.17392839079023448 0.10721918628243715 0.5324896555044976
+ 0.2294970198210603 0.1475713493722641 0.21732047829578108
+ 0.3411526299085336 0.30826408258696447 0.2179924118612528
+ 0.2207344248758067 0.2739325898731973 0.18839036800196632
+ 0.17782963637925117 0.32966429276894926 0.3582051521191558
+ 0.39562921531279693 0.1499968776598779 0.2505894375812506
+ 0.4326928026455318 0.17738690973927634 0.3462976492699658
+ 0.23395102530403086 0.2966693183426996 0.5496857078634017
+ 0.44297368061046904 0.474792939435385 0.1329719426790843
+ 0.29228166672500194 0.20585032553961732 0.16035337350148743
+ 0.2646505042905001 0.4633522072833276 0.24670734972568606
+ 0.2217962750785699 0.3803720763559033 0.30759743662392103
+ 0.37230916454385327 0.2405882081553286 0.21118955983996365
+ 0.3914908422393354 0.3943451019642236 0.19811359031408235
+ 0.5032897493761714 0.2373133580609201 0.4818693338503306]</t>
+  </si>
+  <si>
+    <t>4      0.0736294
+5       0.112262
+6      0.0646102
+7      0.0484941
+8      0.0981734
+         ...    
+362    0.0720497
+363     0.150292
+364    0.0757686
+365    0.0434911
+366    0.0525857
+Length: 336, dtype: object</t>
+  </si>
+  <si>
+    <t>4      0.135886
+5      0.194547
+6      0.177083
+7      0.197035
+8      0.219865
+         ...   
+362    0.162016
+363    0.247784
+364    0.149688
+365    0.184546
+366    0.131382
+Length: 336, dtype: object</t>
+  </si>
+  <si>
+    <t>4      0.269872
+5      0.324936
+6      0.305051
+7      0.209501
+8      0.248602
+         ...   
+362    0.244458
+363     0.25532
+364     0.17152
+365     0.41671
+366    0.228144
+Length: 336, dtype: object</t>
+  </si>
+  <si>
+    <t>4       0.104994
+5       0.134204
+6      0.0984491
+7       0.152391
+8       0.168353
+         ...    
+362     0.127131
+363     0.148491
+364    0.0997336
+365      0.11794
+366      0.10602
+Length: 336, dtype: object</t>
   </si>
 </sst>
 </file>
@@ -476,13 +556,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AH2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:34">
+    <row r="1" spans="1:6">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -498,172 +578,25 @@
       <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="E2" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="F2" t="s">
         <v>9</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:34">
-      <c r="A2" s="1">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F2">
-        <v>9440410.16</v>
-      </c>
-      <c r="G2">
-        <v>0.063928115047806</v>
-      </c>
-      <c r="H2">
-        <v>10484</v>
-      </c>
-      <c r="I2">
-        <v>0.988963305348552</v>
-      </c>
-      <c r="K2">
-        <v>2968004.7</v>
-      </c>
-      <c r="L2">
-        <v>0.03922865262361954</v>
-      </c>
-      <c r="M2">
-        <v>11707</v>
-      </c>
-      <c r="N2">
-        <v>0.9031088482604336</v>
-      </c>
-      <c r="P2">
-        <v>4755520.72</v>
-      </c>
-      <c r="Q2">
-        <v>0.0491609885753445</v>
-      </c>
-      <c r="R2">
-        <v>21285</v>
-      </c>
-      <c r="S2">
-        <v>0.9773175995224758</v>
-      </c>
-      <c r="U2">
-        <v>7069200.41</v>
-      </c>
-      <c r="V2">
-        <v>0.03697623503743152</v>
-      </c>
-      <c r="W2">
-        <v>5964</v>
-      </c>
-      <c r="X2">
-        <v>0.9444180522565321</v>
-      </c>
-      <c r="Z2">
-        <v>3837432.13</v>
-      </c>
-      <c r="AA2">
-        <v>0.04960923617030877</v>
-      </c>
-      <c r="AB2">
-        <v>7973</v>
-      </c>
-      <c r="AC2">
-        <v>0.4409113532046673</v>
-      </c>
-      <c r="AE2">
-        <v>28070568.12</v>
-      </c>
-      <c r="AF2">
-        <v>0.04769036126202952</v>
-      </c>
-      <c r="AG2">
-        <v>57413</v>
-      </c>
-      <c r="AH2">
-        <v>0.8232316714701539</v>
       </c>
     </row>
   </sheetData>

</xml_diff>